<commit_message>
Deployed dfeae72 with MkDocs version: 1.4.1
</commit_message>
<xml_diff>
--- a/rootme/web-server/db.xlsx
+++ b/rootme/web-server/db.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_study\01_self\01_web\01_blog\main\hieuhdh.github.io\docs\rootme\web-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF429D82-2F83-4DF4-8931-1C332915E1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A7860-3C62-4888-801A-121EB94A8E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_sql_injection" sheetId="1" r:id="rId1"/>
+    <sheet name="_php" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Tên Challenge</t>
   </si>
@@ -103,13 +104,79 @@
   </si>
   <si>
     <t>https://www.root-me.org/en/Challenges/Web-Server/SQL-injection-Filter-bypass</t>
+  </si>
+  <si>
+    <t>Local File Inclusion</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/Local-File-Inclusion</t>
+  </si>
+  <si>
+    <t>Local File Inclusion - Double encoding</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/Local-File-Inclusion-Double-encoding</t>
+  </si>
+  <si>
+    <t>Local File Inclusion - Wrappers</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/Local-File-Inclusion-Wrappers</t>
+  </si>
+  <si>
+    <t>Remote File Inclusion</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/Remote-File-Inclusion</t>
+  </si>
+  <si>
+    <t>HTTP - Directory indexing</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/HTTP-Directory-indexing</t>
+  </si>
+  <si>
+    <t>File upload - Double extensions</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/File-upload-Double-extensions</t>
+  </si>
+  <si>
+    <t>File upload - MIME type</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/File-upload-MIME-type</t>
+  </si>
+  <si>
+    <t>Directory traversal</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/Directory-traversal</t>
+  </si>
+  <si>
+    <t>PHP - assert()</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/PHP-assert</t>
+  </si>
+  <si>
+    <t>PHP - Filters</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/PHP-Filters</t>
+  </si>
+  <si>
+    <t>PHP - register globals</t>
+  </si>
+  <si>
+    <t>https://www.root-me.org/en/Challenges/Web-Server/PHP-register-globals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +189,27 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,14 +229,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -548,4 +643,122 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3081A19A-D121-4DE5-89C5-400F03B2AA6E}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="133" customWidth="1"/>
+    <col min="2" max="2" width="76" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{295FA552-D15F-4F9E-8CCB-7E2CCB9DBEA5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>